<commit_message>
Make small fix to template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -325,8 +325,7 @@
     <col customWidth="1" min="4" max="4" width="5.86"/>
     <col customWidth="1" min="6" max="6" width="37.0"/>
     <col customWidth="1" min="7" max="7" width="10.14"/>
-    <col customWidth="1" min="8" max="8" width="7.0"/>
-    <col customWidth="1" min="9" max="9" width="5.86"/>
+    <col customWidth="1" min="8" max="9" width="7.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -963,15 +962,15 @@
         <v>3</v>
       </c>
       <c r="G22" s="4" t="str">
-        <f>ROUND(AVERAGE(OpenJDK_TIME!A1:A1009),3)</f>
+        <f t="shared" ref="G22:I22" si="2">ROUND(AVERAGE(OpenJDK_TIME!A1:A1009),5)</f>
         <v>#REF!</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f>ROUND(AVERAGE(OpenJDK_TIME!B1:B1009),5)</f>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f>ROUND(AVERAGE(OpenJDK_TIME!C1:C1009),0)</f>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N22" s="3"/>
@@ -993,15 +992,15 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="str">
-        <f t="shared" ref="B23:D23" si="2">MEDIAN(GraalVM_TIME!A1:A1009)</f>
+        <f t="shared" ref="B23:D23" si="3">MEDIAN(GraalVM_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="C23" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
       <c r="E23" s="3"/>
@@ -1009,15 +1008,15 @@
         <v>4</v>
       </c>
       <c r="G23" s="4" t="str">
-        <f t="shared" ref="G23:I23" si="3">MEDIAN(OpenJDK_TIME!A1:A1009)</f>
+        <f t="shared" ref="G23:I23" si="4">MEDIAN(OpenJDK_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="N23" s="3"/>
@@ -1039,15 +1038,15 @@
         <v>5</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f t="shared" ref="B24:D24" si="4">MIN(GraalVM_TIME!A1:A1009)</f>
+        <f t="shared" ref="B24:D24" si="5">MIN(GraalVM_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="C24" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
       <c r="E24" s="3"/>
@@ -1055,15 +1054,15 @@
         <v>5</v>
       </c>
       <c r="G24" s="4" t="str">
-        <f t="shared" ref="G24:I24" si="5">MIN(OpenJDK_TIME!A1:A1009)</f>
+        <f t="shared" ref="G24:I24" si="6">MIN(OpenJDK_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="N24" s="3"/>
@@ -1085,15 +1084,15 @@
         <v>6</v>
       </c>
       <c r="B25" s="3" t="str">
-        <f t="shared" ref="B25:D25" si="6">MAX(GraalVM_TIME!A1:A1009)</f>
+        <f t="shared" ref="B25:D25" si="7">MAX(GraalVM_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="C25" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
       <c r="E25" s="3"/>
@@ -1101,15 +1100,15 @@
         <v>6</v>
       </c>
       <c r="G25" s="4" t="str">
-        <f t="shared" ref="G25:I25" si="7">MAX(OpenJDK_TIME!A1:A1009)</f>
+        <f t="shared" ref="G25:I25" si="8">MAX(OpenJDK_TIME!A1:A1009)</f>
         <v>#REF!</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="N25" s="3"/>

</xml_diff>